<commit_message>
modified excel file for easier use in matlab
</commit_message>
<xml_diff>
--- a/AP_results.xlsx
+++ b/AP_results.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katie\Desktop\BME504 Project\TES model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ryan/Desktop/Duke/neuron/nmbmodel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11472" windowHeight="4032" xr2:uid="{F946F00B-7C1D-4AAD-9B95-01473EB90F8E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>A</t>
   </si>
@@ -44,46 +50,13 @@
     <t>J</t>
   </si>
   <si>
-    <t>1 mA</t>
-  </si>
-  <si>
-    <t>1.75 mA</t>
-  </si>
-  <si>
-    <t>2.5 mA</t>
-  </si>
-  <si>
-    <t>3 mA</t>
-  </si>
-  <si>
-    <t>3.75mA</t>
-  </si>
-  <si>
-    <t>4.25 mA</t>
-  </si>
-  <si>
-    <t>5 mA</t>
-  </si>
-  <si>
-    <t>7.5 mA</t>
-  </si>
-  <si>
-    <t>10 mA</t>
-  </si>
-  <si>
-    <t>12.5 mA</t>
-  </si>
-  <si>
-    <t>15 mA</t>
-  </si>
-  <si>
-    <t>17.5 mA</t>
+    <t>Current (mA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +74,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -111,116 +84,116 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -228,10 +201,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -239,49 +212,49 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -289,61 +262,61 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -351,14 +324,51 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -366,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -374,17 +384,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,14 +405,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,68 +751,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96DBA96-0B20-4FA6-8DF1-60BFEB0946CC}">
-  <dimension ref="D2:Q23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="13" t="s">
+    <row r="1" spans="4:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="4:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="7" t="s">
+      <c r="F3" s="22">
+        <v>1</v>
+      </c>
+      <c r="G3" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="H3" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="I3" s="23">
+        <v>3</v>
+      </c>
+      <c r="J3" s="23">
+        <v>3.75</v>
+      </c>
+      <c r="K3" s="23">
+        <v>4.25</v>
+      </c>
+      <c r="L3" s="23">
+        <v>5</v>
+      </c>
+      <c r="M3" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="N3" s="23">
         <v>10</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="23">
+        <v>12.5</v>
+      </c>
+      <c r="P3" s="23">
         <v>15</v>
       </c>
-      <c r="P3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
+      <c r="Q3" s="24">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
         <v>0</v>
       </c>
       <c r="G4" s="2">
@@ -814,12 +865,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D5" s="19"/>
-      <c r="E5" s="15">
+    <row r="5" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D5" s="14"/>
+      <c r="E5" s="20">
         <v>0.1</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <v>0</v>
       </c>
       <c r="G5" s="1">
@@ -856,12 +907,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D6" s="19"/>
-      <c r="E6" s="15">
+    <row r="6" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D6" s="14"/>
+      <c r="E6" s="20">
         <v>0.3</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>0</v>
       </c>
       <c r="G6" s="1">
@@ -898,12 +949,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D7" s="19"/>
-      <c r="E7" s="15">
+    <row r="7" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D7" s="14"/>
+      <c r="E7" s="20">
         <v>0.5</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>0</v>
       </c>
       <c r="G7" s="1">
@@ -940,12 +991,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="20"/>
-      <c r="E8" s="16">
-        <v>1</v>
-      </c>
-      <c r="F8" s="12">
+    <row r="8" spans="4:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="15"/>
+      <c r="E8" s="21">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
         <v>0</v>
       </c>
       <c r="G8" s="5">
@@ -982,14 +1033,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D9" s="21" t="s">
+    <row r="9" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="14">
-        <v>0</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="E9" s="19">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
         <v>0</v>
       </c>
       <c r="G9" s="2">
@@ -1026,12 +1077,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D10" s="22"/>
-      <c r="E10" s="15">
+    <row r="10" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D10" s="11"/>
+      <c r="E10" s="20">
         <v>0.1</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <v>0</v>
       </c>
       <c r="G10" s="1">
@@ -1068,12 +1119,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D11" s="22"/>
-      <c r="E11" s="15">
+    <row r="11" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D11" s="11"/>
+      <c r="E11" s="20">
         <v>0.3</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>0</v>
       </c>
       <c r="G11" s="1">
@@ -1110,12 +1161,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D12" s="22"/>
-      <c r="E12" s="15">
+    <row r="12" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D12" s="11"/>
+      <c r="E12" s="20">
         <v>0.5</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>0</v>
       </c>
       <c r="G12" s="1">
@@ -1152,12 +1203,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="23"/>
-      <c r="E13" s="16">
-        <v>1</v>
-      </c>
-      <c r="F13" s="12">
+    <row r="13" spans="4:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="12"/>
+      <c r="E13" s="21">
+        <v>1</v>
+      </c>
+      <c r="F13" s="9">
         <v>0</v>
       </c>
       <c r="G13" s="5">
@@ -1194,14 +1245,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D14" s="21" t="s">
+    <row r="14" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D14" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10">
+      <c r="E14" s="19">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
         <v>0</v>
       </c>
       <c r="G14" s="2">
@@ -1238,12 +1289,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D15" s="22"/>
-      <c r="E15" s="15">
+    <row r="15" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D15" s="11"/>
+      <c r="E15" s="20">
         <v>0.1</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <v>0</v>
       </c>
       <c r="G15" s="1">
@@ -1280,12 +1331,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D16" s="22"/>
-      <c r="E16" s="15">
+    <row r="16" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D16" s="11"/>
+      <c r="E16" s="20">
         <v>0.3</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <v>0</v>
       </c>
       <c r="G16" s="1">
@@ -1322,12 +1373,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D17" s="22"/>
-      <c r="E17" s="15">
+    <row r="17" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D17" s="11"/>
+      <c r="E17" s="20">
         <v>0.5</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>0</v>
       </c>
       <c r="G17" s="1">
@@ -1364,12 +1415,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="23"/>
-      <c r="E18" s="16">
-        <v>1</v>
-      </c>
-      <c r="F18" s="12">
+    <row r="18" spans="4:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="12"/>
+      <c r="E18" s="21">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
         <v>0</v>
       </c>
       <c r="G18" s="5">
@@ -1406,14 +1457,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D19" s="21" t="s">
+    <row r="19" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="14">
-        <v>0</v>
-      </c>
-      <c r="F19" s="10">
+      <c r="E19" s="19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
         <v>0</v>
       </c>
       <c r="G19" s="2">
@@ -1450,12 +1501,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D20" s="22"/>
-      <c r="E20" s="15">
+    <row r="20" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D20" s="11"/>
+      <c r="E20" s="20">
         <v>0.1</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8">
         <v>0</v>
       </c>
       <c r="G20" s="1">
@@ -1492,12 +1543,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D21" s="22"/>
-      <c r="E21" s="15">
+    <row r="21" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D21" s="11"/>
+      <c r="E21" s="20">
         <v>0.3</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="8">
         <v>0</v>
       </c>
       <c r="G21" s="1">
@@ -1534,12 +1585,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D22" s="22"/>
-      <c r="E22" s="15">
+    <row r="22" spans="4:17" x14ac:dyDescent="0.2">
+      <c r="D22" s="11"/>
+      <c r="E22" s="20">
         <v>0.5</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="8">
         <v>0</v>
       </c>
       <c r="G22" s="1">
@@ -1576,12 +1627,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="4:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="23"/>
-      <c r="E23" s="16">
-        <v>1</v>
-      </c>
-      <c r="F23" s="12">
+    <row r="23" spans="4:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="12"/>
+      <c r="E23" s="21">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9">
         <v>0</v>
       </c>
       <c r="G23" s="5">
@@ -1619,11 +1670,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D19:D23"/>
     <mergeCell ref="D14:D18"/>
     <mergeCell ref="D9:D13"/>
     <mergeCell ref="D4:D8"/>
+    <mergeCell ref="F2:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:Q23">
     <cfRule type="colorScale" priority="1">

</xml_diff>